<commit_message>
#102 Group 4 Assignment 4 (final version)
Comments added
</commit_message>
<xml_diff>
--- a/Lecture_4/Assigment_4/output/sbs/group4/table_alfin.xlsx
+++ b/Lecture_4/Assigment_4/output/sbs/group4/table_alfin.xlsx
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -465,12 +465,12 @@
         <v>19</v>
       </c>
       <c r="E2">
-        <v>184.57</v>
+        <v>191.41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -482,12 +482,12 @@
         <v>19</v>
       </c>
       <c r="E3">
-        <v>185.08</v>
+        <v>191.41</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -516,12 +516,12 @@
         <v>19</v>
       </c>
       <c r="E5">
-        <v>191.41</v>
+        <v>185.08</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -533,12 +533,12 @@
         <v>19</v>
       </c>
       <c r="E6">
-        <v>191.41</v>
+        <v>184.57</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -550,12 +550,12 @@
         <v>19</v>
       </c>
       <c r="E7">
-        <v>183.96</v>
+        <v>184.23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -567,7 +567,7 @@
         <v>19</v>
       </c>
       <c r="E8">
-        <v>184.04</v>
+        <v>184.23</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -589,7 +589,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -601,12 +601,12 @@
         <v>19</v>
       </c>
       <c r="E10">
-        <v>184.23</v>
+        <v>184.04</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -618,12 +618,12 @@
         <v>19</v>
       </c>
       <c r="E11">
-        <v>184.23</v>
+        <v>183.96</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -635,12 +635,12 @@
         <v>19</v>
       </c>
       <c r="E12">
-        <v>219.3</v>
+        <v>221.2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -652,7 +652,7 @@
         <v>19</v>
       </c>
       <c r="E13">
-        <v>220.15</v>
+        <v>221.2</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -674,7 +674,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -686,12 +686,12 @@
         <v>19</v>
       </c>
       <c r="E15">
-        <v>221.2</v>
+        <v>220.15</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -703,12 +703,12 @@
         <v>19</v>
       </c>
       <c r="E16">
-        <v>221.2</v>
+        <v>219.3</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -720,12 +720,12 @@
         <v>19</v>
       </c>
       <c r="E17">
-        <v>212.88</v>
+        <v>215.04</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -737,7 +737,7 @@
         <v>19</v>
       </c>
       <c r="E18">
-        <v>212.88</v>
+        <v>214.34</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -759,7 +759,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -771,12 +771,12 @@
         <v>19</v>
       </c>
       <c r="E20">
-        <v>214.34</v>
+        <v>212.88</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -788,12 +788,12 @@
         <v>19</v>
       </c>
       <c r="E21">
-        <v>215.04</v>
+        <v>212.88</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -805,12 +805,12 @@
         <v>19</v>
       </c>
       <c r="E22">
-        <v>165.4</v>
+        <v>181.44</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -822,7 +822,7 @@
         <v>19</v>
       </c>
       <c r="E23">
-        <v>167.69</v>
+        <v>179.75</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -844,7 +844,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -856,12 +856,12 @@
         <v>19</v>
       </c>
       <c r="E25">
-        <v>179.75</v>
+        <v>167.69</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -873,12 +873,12 @@
         <v>19</v>
       </c>
       <c r="E26">
-        <v>181.44</v>
+        <v>165.4</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -890,12 +890,12 @@
         <v>19</v>
       </c>
       <c r="E27">
-        <v>203.69</v>
+        <v>229.88</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
@@ -907,7 +907,7 @@
         <v>19</v>
       </c>
       <c r="E28">
-        <v>205.55</v>
+        <v>222.01</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -929,7 +929,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
@@ -941,12 +941,12 @@
         <v>19</v>
       </c>
       <c r="E30">
-        <v>222.01</v>
+        <v>205.55</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
@@ -958,12 +958,12 @@
         <v>19</v>
       </c>
       <c r="E31">
-        <v>229.88</v>
+        <v>203.69</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -975,12 +975,12 @@
         <v>19</v>
       </c>
       <c r="E32">
-        <v>231.28</v>
+        <v>233.65</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -992,7 +992,7 @@
         <v>19</v>
       </c>
       <c r="E33">
-        <v>232.09</v>
+        <v>232.32</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1014,7 +1014,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -1026,12 +1026,12 @@
         <v>19</v>
       </c>
       <c r="E35">
-        <v>232.32</v>
+        <v>232.09</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -1043,12 +1043,12 @@
         <v>19</v>
       </c>
       <c r="E36">
-        <v>233.65</v>
+        <v>231.28</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -1060,12 +1060,12 @@
         <v>19</v>
       </c>
       <c r="E37">
-        <v>146.52</v>
+        <v>217.99</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -1077,7 +1077,7 @@
         <v>19</v>
       </c>
       <c r="E38">
-        <v>192.29</v>
+        <v>216.81</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1099,7 +1099,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -1111,12 +1111,12 @@
         <v>19</v>
       </c>
       <c r="E40">
-        <v>216.81</v>
+        <v>192.29</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -1128,12 +1128,12 @@
         <v>19</v>
       </c>
       <c r="E41">
-        <v>217.99</v>
+        <v>146.52</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -1145,12 +1145,12 @@
         <v>19</v>
       </c>
       <c r="E42">
-        <v>149.36</v>
+        <v>149.92</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
@@ -1162,7 +1162,7 @@
         <v>19</v>
       </c>
       <c r="E43">
-        <v>149.48</v>
+        <v>149.83</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1184,7 +1184,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -1196,12 +1196,12 @@
         <v>19</v>
       </c>
       <c r="E45">
-        <v>149.83</v>
+        <v>149.48</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
@@ -1213,12 +1213,12 @@
         <v>19</v>
       </c>
       <c r="E46">
-        <v>149.92</v>
+        <v>149.36</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
@@ -1230,12 +1230,12 @@
         <v>19</v>
       </c>
       <c r="E47">
-        <v>150.1</v>
+        <v>150.99</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
@@ -1247,7 +1247,7 @@
         <v>19</v>
       </c>
       <c r="E48">
-        <v>150.29</v>
+        <v>150.95</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1269,7 +1269,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -1281,12 +1281,12 @@
         <v>19</v>
       </c>
       <c r="E50">
-        <v>150.95</v>
+        <v>150.29</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
@@ -1298,12 +1298,12 @@
         <v>19</v>
       </c>
       <c r="E51">
-        <v>150.99</v>
+        <v>150.1</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
@@ -1315,12 +1315,12 @@
         <v>19</v>
       </c>
       <c r="E52">
-        <v>151.29</v>
+        <v>153.05</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
@@ -1332,7 +1332,7 @@
         <v>19</v>
       </c>
       <c r="E53">
-        <v>151.37</v>
+        <v>152.75</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1354,7 +1354,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
         <v>14</v>
@@ -1366,12 +1366,12 @@
         <v>19</v>
       </c>
       <c r="E55">
-        <v>152.75</v>
+        <v>151.37</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
         <v>14</v>
@@ -1383,12 +1383,12 @@
         <v>19</v>
       </c>
       <c r="E56">
-        <v>153.05</v>
+        <v>151.29</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
@@ -1400,12 +1400,12 @@
         <v>19</v>
       </c>
       <c r="E57">
-        <v>152.71</v>
+        <v>153.06</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
@@ -1417,7 +1417,7 @@
         <v>19</v>
       </c>
       <c r="E58">
-        <v>153.03</v>
+        <v>153.06</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1439,7 +1439,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -1451,12 +1451,12 @@
         <v>19</v>
       </c>
       <c r="E60">
-        <v>153.06</v>
+        <v>153.03</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -1468,12 +1468,12 @@
         <v>19</v>
       </c>
       <c r="E61">
-        <v>153.06</v>
+        <v>152.71</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
         <v>16</v>
@@ -1485,12 +1485,12 @@
         <v>19</v>
       </c>
       <c r="E62">
-        <v>151.98</v>
+        <v>152.19</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
         <v>16</v>
@@ -1502,7 +1502,7 @@
         <v>19</v>
       </c>
       <c r="E63">
-        <v>151.99</v>
+        <v>152.16</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1524,7 +1524,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
         <v>16</v>
@@ -1536,12 +1536,12 @@
         <v>19</v>
       </c>
       <c r="E65">
-        <v>152.16</v>
+        <v>151.99</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
         <v>16</v>
@@ -1553,12 +1553,12 @@
         <v>19</v>
       </c>
       <c r="E66">
-        <v>152.19</v>
+        <v>151.98</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B67" t="s">
         <v>17</v>
@@ -1570,12 +1570,12 @@
         <v>19</v>
       </c>
       <c r="E67">
-        <v>149.35</v>
+        <v>152.56</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
         <v>17</v>
@@ -1587,7 +1587,7 @@
         <v>19</v>
       </c>
       <c r="E68">
-        <v>152.21</v>
+        <v>152.32</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1609,7 +1609,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B70" t="s">
         <v>17</v>
@@ -1621,12 +1621,12 @@
         <v>19</v>
       </c>
       <c r="E70">
-        <v>152.32</v>
+        <v>152.21</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
         <v>17</v>
@@ -1638,7 +1638,7 @@
         <v>19</v>
       </c>
       <c r="E71">
-        <v>152.56</v>
+        <v>149.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>